<commit_message>
Update bayesian networks generation code, change the output data format
</commit_message>
<xml_diff>
--- a/output/edges.xlsx
+++ b/output/edges.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Node1</t>
+          <t>Parent_Node</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Node2</t>
+          <t>Child_Node</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P3_STATE</t>
+          <t>P401.Status</t>
         </is>
       </c>
     </row>
@@ -484,36 +484,36 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P2_STATE</t>
+          <t>P101.Status</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P6_STATE</t>
+          <t>P3_STATE</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MV201.Status</t>
+          <t>P2_STATE</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P205.Status</t>
+          <t>P1_STATE</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P201.Status</t>
+          <t>MV201.Status</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FIT201.Pv</t>
+          <t>P203.Status</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AIT303.Pv</t>
+          <t>P205.Status</t>
         </is>
       </c>
     </row>
@@ -556,24 +556,24 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P205.Status</t>
+          <t>P203.Status</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P203.Status</t>
+          <t>FIT201.Pv</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>P3_STATE</t>
+          <t>P205.Status</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MV302.Status</t>
+          <t>AIT303.Pv</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P301.Status</t>
+          <t>MV302.Status</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P401.Status</t>
+          <t>P301.Status</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DPIT301.Pv</t>
+          <t>P3_STATE</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>FIT503.Pv</t>
+          <t>P1_STATE</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P1_STATE</t>
+          <t>P101.Status</t>
         </is>
       </c>
     </row>
@@ -789,19 +789,19 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P101.Status</t>
+          <t>MV201.Status</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>P301.Status</t>
+          <t>P401.Status</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MV201.Status</t>
+          <t>UV401.Status</t>
         </is>
       </c>
     </row>
@@ -813,19 +813,19 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>UV401.Status</t>
+          <t>P5_STATE</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>P401.Status</t>
+          <t>UV401.Status</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P5_STATE</t>
+          <t>FIT503.Pv</t>
         </is>
       </c>
     </row>
@@ -837,19 +837,19 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FIT503.Pv</t>
+          <t>AIT504.Pv</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>UV401.Status</t>
+          <t>P5_STATE</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>AIT504.Pv</t>
+          <t>MV502.Status</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MV501.Status</t>
+          <t>MV504.Status</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MV504.Status</t>
+          <t>MV503.Status</t>
         </is>
       </c>
     </row>
@@ -885,31 +885,31 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MV503.Status</t>
+          <t>P6_STATE</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>P5_STATE</t>
+          <t>FIT503.Pv</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P2_STATE</t>
+          <t>P501.Status</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>FIT503.Pv</t>
+          <t>AIT503.Pv</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P501.Status</t>
+          <t>P101.Status</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P101.Status</t>
+          <t>LSH601.Alarm</t>
         </is>
       </c>
     </row>
@@ -933,31 +933,31 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>LSH601.Alarm</t>
+          <t>P601.Status</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>AIT503.Pv</t>
+          <t>PIT502.Pv</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P601.Status</t>
+          <t>MV501.Status</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>P501.Status</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
           <t>PIT502.Pv</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>MV502.Status</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>PIT502.Pv</t>
+          <t>FIT401.Pv</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>FIT401.Pv</t>
+          <t>PIT501.Pv</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>PIT501.Pv</t>
+          <t>PIT503.Pv</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>PIT503.Pv</t>
+          <t>FIT501.Pv</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>FIT501.Pv</t>
+          <t>FIT502.Pv</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>FIT502.Pv</t>
+          <t>AIT503.Pv</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>AIT503.Pv</t>
+          <t>AIT502.Pv</t>
         </is>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>AIT502.Pv</t>
+          <t>DPIT301.Pv</t>
         </is>
       </c>
     </row>
@@ -1065,55 +1065,55 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>AIT301.Pv</t>
+          <t>P3_STATE</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>MV502.Status</t>
+          <t>P501.Status</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P5_STATE</t>
+          <t>AIT301.Pv</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>P6_STATE</t>
+          <t>MV501.Status</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P1_STATE</t>
+          <t>P5_STATE</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>P601.Status</t>
+          <t>P6_STATE</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P1_STATE</t>
+          <t>P2_STATE</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>LSH601.Alarm</t>
+          <t>P601.Status</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>PIT502.Pv</t>
+          <t>P1_STATE</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>AIT504.Pv</t>
+          <t>PIT502.Pv</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>P1_STATE</t>
+          <t>P3_STATE</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,31 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>P205.Status</t>
+          <t>AIT504.Pv</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>LSH601.Alarm</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>P1_STATE</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>LSH601.Alarm</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>P203.Status</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Produce analyze output, add a new data source, add detailed comments, Update README.md
</commit_message>
<xml_diff>
--- a/output/edges.xlsx
+++ b/output/edges.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,24 +448,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FIT101.Pv</t>
+          <t>P101.Status</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MV101.Status</t>
+          <t>MV201.Status</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MV101.Status</t>
+          <t>P101.Status</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P401.Status</t>
+          <t>P601.Status</t>
         </is>
       </c>
     </row>
@@ -477,19 +477,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MV201.Status</t>
+          <t>P3_STATE</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P101.Status</t>
+          <t>P2_STATE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P3_STATE</t>
+          <t>P6_STATE</t>
         </is>
       </c>
     </row>
@@ -532,12 +532,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>P203.Status</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>P201.Status</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>AIT201.Pv</t>
         </is>
       </c>
     </row>
@@ -549,19 +549,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P201.Status</t>
+          <t>AIT203.Pv</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P203.Status</t>
+          <t>P205.Status</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>FIT201.Pv</t>
+          <t>AIT201.Pv</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AIT303.Pv</t>
+          <t>FIT201.Pv</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MV304.Status</t>
+          <t>AIT503.Pv</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MV303.Status</t>
+          <t>P5_STATE</t>
         </is>
       </c>
     </row>
@@ -621,31 +621,31 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MV301.Status</t>
+          <t>UV401.Status</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DPIT301.Pv</t>
+          <t>P3_STATE</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P301.Status</t>
+          <t>MV304.Status</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MV301.Status</t>
+          <t>DPIT301.Pv</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P602.Status</t>
+          <t>P301.Status</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>FIT301.Pv</t>
+          <t>AIT303.Pv</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AIT503.Pv</t>
+          <t>PIT503.Pv</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>AIT302.Pv</t>
+          <t>PIT501.Pv</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>PIT503.Pv</t>
+          <t>FIT301.Pv</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>PIT502.Pv</t>
+          <t>FIT503.Pv</t>
         </is>
       </c>
     </row>
@@ -729,451 +729,199 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>AIT501.Pv</t>
+          <t>AIT302.Pv</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>P301.Status</t>
+          <t>P4_STATE</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>PIT501.Pv</t>
+          <t>P401.Status</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>P301.Status</t>
+          <t>P4_STATE</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>FIT601.Pv</t>
+          <t>P2_STATE</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>P301.Status</t>
+          <t>UV401.Status</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P1_STATE</t>
+          <t>P4_STATE</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>P301.Status</t>
+          <t>P5_STATE</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P101.Status</t>
+          <t>MV502.Status</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>P301.Status</t>
+          <t>P5_STATE</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MV201.Status</t>
+          <t>MV501.Status</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>P401.Status</t>
+          <t>P5_STATE</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>UV401.Status</t>
+          <t>P501.Status</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>P401.Status</t>
+          <t>P5_STATE</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P5_STATE</t>
+          <t>MV504.Status</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>UV401.Status</t>
+          <t>P5_STATE</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FIT503.Pv</t>
+          <t>MV503.Status</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>UV401.Status</t>
+          <t>AIT503.Pv</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>AIT504.Pv</t>
+          <t>P601.Status</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>P5_STATE</t>
+          <t>PIT501.Pv</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MV502.Status</t>
+          <t>P101.Status</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>P5_STATE</t>
+          <t>P501.Status</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MV504.Status</t>
+          <t>PIT502.Pv</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>P5_STATE</t>
+          <t>P501.Status</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MV503.Status</t>
+          <t>FIT503.Pv</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>P5_STATE</t>
+          <t>P501.Status</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P6_STATE</t>
+          <t>FIT401.Pv</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>FIT503.Pv</t>
+          <t>P501.Status</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P501.Status</t>
+          <t>FIT501.Pv</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>AIT503.Pv</t>
+          <t>P501.Status</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P101.Status</t>
+          <t>AIT504.Pv</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>AIT503.Pv</t>
+          <t>MV503.Status</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>LSH601.Alarm</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>AIT503.Pv</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>P601.Status</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>PIT502.Pv</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>MV501.Status</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>P501.Status</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>PIT502.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>P501.Status</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>FIT401.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>P501.Status</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>PIT501.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>P501.Status</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>PIT503.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>P501.Status</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>FIT501.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>P501.Status</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>FIT502.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>P501.Status</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>AIT503.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>P501.Status</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>AIT502.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>P501.Status</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>DPIT301.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>P501.Status</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>P3_STATE</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>P501.Status</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>AIT301.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>MV501.Status</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>P5_STATE</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>P6_STATE</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>P2_STATE</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>P601.Status</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>P1_STATE</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>LSH601.Alarm</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>PIT502.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>LSH601.Alarm</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>P3_STATE</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>LSH601.Alarm</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>AIT504.Pv</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>LSH601.Alarm</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>P1_STATE</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>LSH601.Alarm</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>P203.Status</t>
+          <t>P4_STATE</t>
         </is>
       </c>
     </row>

</xml_diff>